<commit_message>
Ingresa al SCT, cambia de cuit al representado y descarga el Excel de deudas.
</commit_message>
<xml_diff>
--- a/data/input/clientes.xlsx
+++ b/data/input/clientes.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968CA15C-E115-49A3-994F-BA1E84B4504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2865CF5-DF5E-4378-B611-9C25EEB48187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2415" windowWidth="20490" windowHeight="7635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Contraseña</t>
   </si>
@@ -37,6 +48,12 @@
   </si>
   <si>
     <t>Emilia2023</t>
+  </si>
+  <si>
+    <t>Raiz Descarga</t>
+  </si>
+  <si>
+    <t>Ubicacion Descarga</t>
   </si>
 </sst>
 </file>
@@ -93,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,6 +118,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,9 +414,11 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -404,57 +428,87 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>20246845612</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>30715561227</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="str">
+        <f t="shared" ref="D2:E2" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="E2" s="5" t="str">
+        <f ca="1">D2&amp;"Deudas\"</f>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Descarga el Excel en la ubicacion deseada, luego comprueba si debe descargar otro Excel del mismo cuit a ingresar pero distinto cuit representado y luego comprueba si debe cerrar sesion o no.
</commit_message>
<xml_diff>
--- a/data/input/clientes.xlsx
+++ b/data/input/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2865CF5-DF5E-4378-B611-9C25EEB48187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B71D3A0-92CB-4EE9-8DAB-395BA5C7F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Contraseña</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Ubicacion Descarga</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -83,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,6 +115,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -118,11 +138,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +438,7 @@
     <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -434,81 +454,147 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>20246845612</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>30715561227</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="str">
-        <f t="shared" ref="D2:E2" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
+      <c r="D2" s="3" t="str">
+        <f t="shared" ref="D2:D3" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="3" t="str">
         <f ca="1">D2&amp;"Deudas\"</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5">
+        <f>IF(A2=A1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <f>IF(A2=A3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <f>F2+G2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>20246845612</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20246845612</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f ca="1">D3&amp;"Deudas\"</f>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3" si="1">IF(A3=A2,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3" si="2">IF(A3=A4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3" si="3">F3+G3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extrae el Excel y la cantidad de faltas de presentacion de manera correcta, falta que arme el reporte
</commit_message>
<xml_diff>
--- a/data/input/clientes.xlsx
+++ b/data/input/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B71D3A0-92CB-4EE9-8DAB-395BA5C7F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C820AE5-4BC9-4499-9FCD-61D464948442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Contraseña</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Estudio Rivarossa</t>
+  </si>
+  <si>
+    <t>David Berger</t>
+  </si>
+  <si>
+    <t>Ignacio Zbrun</t>
+  </si>
+  <si>
+    <t>Merentiel2024</t>
   </si>
 </sst>
 </file>
@@ -423,178 +438,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
         <v>20246845612</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>30715561227</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D3" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
+      <c r="E2" s="3" t="str">
+        <f t="shared" ref="E2:E5" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
       </c>
-      <c r="E2" s="3" t="str">
-        <f ca="1">D2&amp;"Deudas\"</f>
+      <c r="F2" s="3" t="str">
+        <f ca="1">E2&amp;"Deudas\"</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
       </c>
-      <c r="F2" s="5">
-        <f>IF(A2=A1,1,0)</f>
+      <c r="G2" s="5">
+        <f>IF(B2=B1,1,0)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="5">
-        <f>IF(A2=A3,1,0)</f>
+      <c r="H2" s="5">
+        <f>IF(B2=B3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="5">
-        <f>F2+G2</f>
+      <c r="I2" s="5">
+        <f>G2+H2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>20246845612</v>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>20246845612</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>20246845612</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="str">
+      <c r="E3" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
       </c>
-      <c r="E3" s="3" t="str">
-        <f ca="1">D3&amp;"Deudas\"</f>
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F4" ca="1" si="1">E3&amp;"Deudas\"</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
       </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3" si="1">IF(A3=A2,1,0)</f>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G4" si="2">IF(B3=B2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="5">
-        <f t="shared" ref="G3" si="2">IF(A3=A4,1,0)</f>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H4" si="3">IF(B3=B4,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3" si="3">F3+G3</f>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I4" si="4">G3+H3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20434943966</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20434943966</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pruebas realizadas, funciona correctamente
</commit_message>
<xml_diff>
--- a/data/input/clientes.xlsx
+++ b/data/input/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C820AE5-4BC9-4499-9FCD-61D464948442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077F0FD7-1541-4FD5-83C8-2210CFC13A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Contraseña</t>
   </si>
@@ -47,9 +47,6 @@
     <t>CUIT representado</t>
   </si>
   <si>
-    <t>Emilia2023</t>
-  </si>
-  <si>
     <t>Raiz Descarga</t>
   </si>
   <si>
@@ -68,16 +65,44 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Estudio Rivarossa</t>
-  </si>
-  <si>
-    <t>David Berger</t>
-  </si>
-  <si>
-    <t>Ignacio Zbrun</t>
-  </si>
-  <si>
-    <t>Merentiel2024</t>
+    <t xml:space="preserve">((#Urquiza#7411))
+</t>
+  </si>
+  <si>
+    <t>Omarbu2024</t>
+  </si>
+  <si>
+    <t>Alberto2024</t>
+  </si>
+  <si>
+    <t>Estudio2024</t>
+  </si>
+  <si>
+    <t>Marcelo2023</t>
+  </si>
+  <si>
+    <t>Gabriela2023</t>
+  </si>
+  <si>
+    <t>Alfredo Quintana</t>
+  </si>
+  <si>
+    <t>Burgi Omar</t>
+  </si>
+  <si>
+    <t>Fassi Alberto</t>
+  </si>
+  <si>
+    <t>Florentino Rivarossa</t>
+  </si>
+  <si>
+    <t>Seffino Marcelo</t>
+  </si>
+  <si>
+    <t>Gabriela Evangelina Lisi</t>
+  </si>
+  <si>
+    <t>Gabriela Evangelina Lisi y Seffino Marcelo</t>
   </si>
 </sst>
 </file>
@@ -438,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,14 +474,14 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="93.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="101.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -468,36 +493,36 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>20246845612</v>
+        <v>20111155500</v>
       </c>
       <c r="C2" s="1">
-        <v>30715561227</v>
+        <v>20111155500</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" ref="E2:E5" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
+        <f t="shared" ref="E2:E8" ca="1" si="0">LEFT(CELL("filename"),FIND("[",CELL("filename"))-1)</f>
         <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
       </c>
       <c r="F2" s="3" t="str">
@@ -510,25 +535,25 @@
       </c>
       <c r="H2" s="5">
         <f>IF(B2=B3,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="5">
         <f>G2+H2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
-        <v>20246845612</v>
+        <v>20115710037</v>
       </c>
       <c r="C3" s="1">
-        <v>20246845612</v>
+        <v>20115710037</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -540,7 +565,7 @@
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G4" si="2">IF(B3=B2,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H4" si="3">IF(B3=B4,1,0)</f>
@@ -548,21 +573,21 @@
       </c>
       <c r="I3" s="5">
         <f t="shared" ref="I3:I4" si="4">G3+H3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
-        <v>20434943966</v>
+        <v>20170895658</v>
       </c>
       <c r="C4" s="1">
-        <v>20434943966</v>
+        <v>20170895658</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -586,70 +611,140 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20113062518</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20113062518</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f t="shared" ref="F5:F8" ca="1" si="5">E5&amp;"Deudas\"</f>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G8" si="6">IF(B5=B4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ref="H5:H8" si="7">IF(B5=B6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5:I8" si="8">G5+H5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>23163038919</v>
+      </c>
+      <c r="C6" s="1">
+        <v>23163038919</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>23163038919</v>
+      </c>
+      <c r="C7" s="1">
+        <v>30715364170</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>27160314066</v>
+      </c>
+      <c r="C8" s="1">
+        <v>27160314066</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>C:\Program Files\Sublime Merge\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Escritura manual en lugar de automatizada y pausa para ingresar clave
</commit_message>
<xml_diff>
--- a/data/input/clientes.xlsx
+++ b/data/input/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\OneDrive\Escritorio\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E314C02-4EAB-48AF-9FD1-D64F77344998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A261E90-C75E-439A-8230-105E0270CC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cliente</t>
   </si>
@@ -69,15 +69,6 @@
   </si>
   <si>
     <t>C:\Users\ignac\OneDrive\Escritorio\Descarga-masiva-deuda-Sistema-de-Cuentas-Tributarias\data\input\Deudas\</t>
-  </si>
-  <si>
-    <t>Nombre cliente</t>
-  </si>
-  <si>
-    <t>00000000000</t>
-  </si>
-  <si>
-    <t>xxxxxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -133,13 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,17 +434,13 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="104" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -491,37 +476,24 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2">
-        <f>IF(B2=B1, 1, 0)</f>
+      <c r="G2">
+        <f>IF(B1=B2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="2">
-        <f>IF(B2=B3, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2">
+        <f>IF(B2=B3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
         <f>G2+H2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="2"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>